<commit_message>
Continuacao da lista de variaveis
</commit_message>
<xml_diff>
--- a/Lista de variáveis.xlsx
+++ b/Lista de variáveis.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Thabata\Facú\1_2015\Téc Prog\Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thabata\Documents\GitHub\APB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="330">
   <si>
     <t>Class</t>
   </si>
@@ -573,6 +573,447 @@
   </si>
   <si>
     <t>count</t>
+  </si>
+  <si>
+    <t>AgendaDAOTeste</t>
+  </si>
+  <si>
+    <t>PhonebookDAOTest</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>contact1</t>
+  </si>
+  <si>
+    <t>// Instance for a contact from "Phonebook" class</t>
+  </si>
+  <si>
+    <t>contato2</t>
+  </si>
+  <si>
+    <t>contact2</t>
+  </si>
+  <si>
+    <t>// Second instance, for another contact from "Phonebook" class</t>
+  </si>
+  <si>
+    <t>agendaDAO</t>
+  </si>
+  <si>
+    <t>phonebookDAO</t>
+  </si>
+  <si>
+    <t>// Gets the instance from "PhonebookDAO" class</t>
+  </si>
+  <si>
+    <t>getInstanceDeAgendaDAODeveRetonarInstanciaCorrente</t>
+  </si>
+  <si>
+    <t>getInstanceOfPhonebookDAO</t>
+  </si>
+  <si>
+    <t>inserirDeAgendaDAODeveCadastrarUmContato</t>
+  </si>
+  <si>
+    <t>addFromPhonebookDAO</t>
+  </si>
+  <si>
+    <t>// Testing the adding of a new contact</t>
+  </si>
+  <si>
+    <t>excluirDeAgendaDAODeveEnviarUmAgenda</t>
+  </si>
+  <si>
+    <t>deleteFromPhonebookDAO</t>
+  </si>
+  <si>
+    <t>// Testing the deletion of a new contact</t>
+  </si>
+  <si>
+    <t>alterarDeAgendaDAODeveEnviarUmContato</t>
+  </si>
+  <si>
+    <t>editFromPhonebookDAO</t>
+  </si>
+  <si>
+    <t>// Testing the edition of a new contact</t>
+  </si>
+  <si>
+    <t>inserirDeAgendaDAOPassandoUmContatoNulo</t>
+  </si>
+  <si>
+    <t>addFromPhonebookDAOWhenInvalidContact</t>
+  </si>
+  <si>
+    <t>// Testing the adding of a new contact when contact is null</t>
+  </si>
+  <si>
+    <t>excluirDeAgendaDAOPassandoUmContatoNulo</t>
+  </si>
+  <si>
+    <t>deleteFromPhonebookDAOWhenInvalidContact</t>
+  </si>
+  <si>
+    <t>// Testing the deletion of a new contact when contact is null</t>
+  </si>
+  <si>
+    <t>alterarDeAgendaDAOPassandoUmContatoNulo</t>
+  </si>
+  <si>
+    <t>editFromPhonebookDAOWhenInvalidContact</t>
+  </si>
+  <si>
+    <t>// Testing the edition of a new contact when contact is null</t>
+  </si>
+  <si>
+    <t>alterarDeAgendaDAOPassandoUmAgendaAleradoNulo</t>
+  </si>
+  <si>
+    <t>editFromPhonebookDAOWhenEditedNullPhonebook</t>
+  </si>
+  <si>
+    <t>// Testing the edition of a new contact when edited phonebook is null</t>
+  </si>
+  <si>
+    <t>mostrarContatosAgendaDAODeveMostrarContato</t>
+  </si>
+  <si>
+    <t>showPhonebookContactsDAO</t>
+  </si>
+  <si>
+    <t>resultInstance</t>
+  </si>
+  <si>
+    <t>// ResultSet Instance</t>
+  </si>
+  <si>
+    <t>contactName</t>
+  </si>
+  <si>
+    <t>// Shows the contact´s name</t>
+  </si>
+  <si>
+    <t>pesquisaPorNomeDeAgendaDAODeveMostrarContato</t>
+  </si>
+  <si>
+    <t>searchByNameFromPhonebookDAO</t>
+  </si>
+  <si>
+    <t>// Searches the contact´s name</t>
+  </si>
+  <si>
+    <t>pesquisarPorTelefoneDeBarbeiroDAODeveMostrarBarbeiros</t>
+  </si>
+  <si>
+    <t>searchByNumberFromBarberDAO</t>
+  </si>
+  <si>
+    <t>// Receives the contact name to the search</t>
+  </si>
+  <si>
+    <t>BarbeiroControllerTeste</t>
+  </si>
+  <si>
+    <t>BarberControllerTest</t>
+  </si>
+  <si>
+    <t>barberInstance</t>
+  </si>
+  <si>
+    <t>// Instance of the "Barber" class</t>
+  </si>
+  <si>
+    <t>barberData</t>
+  </si>
+  <si>
+    <t>// Receives a variety of data about the barber</t>
+  </si>
+  <si>
+    <t>barbeiroController</t>
+  </si>
+  <si>
+    <t>barberController</t>
+  </si>
+  <si>
+    <t>// Instance of the "BarberController" class</t>
+  </si>
+  <si>
+    <t>getInstanceDeBarbeiroControlerDeveRetonarInstanciaCorrente</t>
+  </si>
+  <si>
+    <t>getInstanceOfBarberController</t>
+  </si>
+  <si>
+    <t>inserirDeBarbeiroControllerDeveEnviarUmBarbeiro</t>
+  </si>
+  <si>
+    <t>addFromBarberController</t>
+  </si>
+  <si>
+    <t>excluirDeBarbeiroControllerDeveEnviarUmBarbeiro</t>
+  </si>
+  <si>
+    <t>deleteFromBarberController</t>
+  </si>
+  <si>
+    <t>alterarDeBarbeiroControllerDeveEnviarUmBarbeiro</t>
+  </si>
+  <si>
+    <t>editFromBarberController</t>
+  </si>
+  <si>
+    <t>barber</t>
+  </si>
+  <si>
+    <t>// Receives the barber´s name to the edit</t>
+  </si>
+  <si>
+    <t>inserirBarbeiroNaoPodePassarBarbeiroNullo</t>
+  </si>
+  <si>
+    <t>addNotNullBarber</t>
+  </si>
+  <si>
+    <t>excluirBarbeiroNaoPodePassarBarbeiroNullo</t>
+  </si>
+  <si>
+    <t>deleteNotNullBarber</t>
+  </si>
+  <si>
+    <t>alterarBarbeiroNaoPodePassarBarbeiroNullo</t>
+  </si>
+  <si>
+    <t>editNotNullBarber</t>
+  </si>
+  <si>
+    <t>procurarPorBarbeiroControllerDeveMostrarUmBarbeiro</t>
+  </si>
+  <si>
+    <t>searchByBarberController</t>
+  </si>
+  <si>
+    <t>mostrarBarbeirosDeBarbeiroControllerDeveMostrarUmBarbeiro</t>
+  </si>
+  <si>
+    <t>displayBarberFromController</t>
+  </si>
+  <si>
+    <t>pesquisarPorNomeDeBarbeiroControllerDeveMostrarUmBarbeiro</t>
+  </si>
+  <si>
+    <t>searchByBarberNameController</t>
+  </si>
+  <si>
+    <t>RelatorioTeste</t>
+  </si>
+  <si>
+    <t>ReportTest</t>
+  </si>
+  <si>
+    <t>relatorio</t>
+  </si>
+  <si>
+    <t>reportInstance</t>
+  </si>
+  <si>
+    <t>// Instance of the "Report" class</t>
+  </si>
+  <si>
+    <t>dataInicialNaoPodeSerSettadaNula</t>
+  </si>
+  <si>
+    <t>initialNotNullDate</t>
+  </si>
+  <si>
+    <t>dataInicialNaoPodeSerSettadaEmBranco</t>
+  </si>
+  <si>
+    <t>initialNotBlankDate</t>
+  </si>
+  <si>
+    <t>dataFinalNaoPodeSerSettadaNula</t>
+  </si>
+  <si>
+    <t>finalNotNullDate</t>
+  </si>
+  <si>
+    <t>dataFinalNaoPodeSerSettaEmBranco</t>
+  </si>
+  <si>
+    <t>finalNotBlankDate</t>
+  </si>
+  <si>
+    <t>barbeiroNaoPodeSerSettadoNulo</t>
+  </si>
+  <si>
+    <t>notNullBarber</t>
+  </si>
+  <si>
+    <t>barbeiroNaoPodeSerSettoEmBranco</t>
+  </si>
+  <si>
+    <t>notBlankBarber</t>
+  </si>
+  <si>
+    <t>tipoDeServicoNaoPodeSerSettadoNulo</t>
+  </si>
+  <si>
+    <t>notNullServiceType</t>
+  </si>
+  <si>
+    <t>tipoDeServicoNaoPodeSerSettoEmBranco</t>
+  </si>
+  <si>
+    <t>notBlankServiceType</t>
+  </si>
+  <si>
+    <t>construtorDeRelatorioNaoPodePassarBarbeiroNulo</t>
+  </si>
+  <si>
+    <t>notNullBarberReportConstructor</t>
+  </si>
+  <si>
+    <t>construtorDeRelatorioNaoPodePassarDataFinalNula</t>
+  </si>
+  <si>
+    <t>notNullFinalDateReportConstructor</t>
+  </si>
+  <si>
+    <t>construtorDeRelatorioNaoPodePassarDataInicialNula</t>
+  </si>
+  <si>
+    <t>notNullInitialDateReportConstructor</t>
+  </si>
+  <si>
+    <t>construtorDeRelatorioNaoPodePassarTipoServicoNulo</t>
+  </si>
+  <si>
+    <t>notNullServiceTypeReportConstructor</t>
+  </si>
+  <si>
+    <t>construtorDeRelatorioPassandoTodosOsDadosCorretos</t>
+  </si>
+  <si>
+    <t>allCorrectReportConstructor</t>
+  </si>
+  <si>
+    <t>// Instance of the "Report" class used in the assertion methods</t>
+  </si>
+  <si>
+    <t>metodoParaTestarGetterDeBarbeiro</t>
+  </si>
+  <si>
+    <t>barberGetterTester</t>
+  </si>
+  <si>
+    <t>metodoParaTestarGetterDeTipoDeServico</t>
+  </si>
+  <si>
+    <t>serviceTypeGetterTester</t>
+  </si>
+  <si>
+    <t>metodoParaTestarGetterDeDataInicial</t>
+  </si>
+  <si>
+    <t>initialDateGetterTester</t>
+  </si>
+  <si>
+    <t>metodoParaTestarGetterDeDataFinal</t>
+  </si>
+  <si>
+    <t>finalDateGetterTester</t>
+  </si>
+  <si>
+    <t>testeDataParaConverter</t>
+  </si>
+  <si>
+    <t>dateToConvertTest</t>
+  </si>
+  <si>
+    <t>TipoServicoControllerTeste</t>
+  </si>
+  <si>
+    <t>ServiceTypeControllerTest</t>
+  </si>
+  <si>
+    <t>servico</t>
+  </si>
+  <si>
+    <t>serviceInstance</t>
+  </si>
+  <si>
+    <t>// Instance of "ServiceType" class</t>
+  </si>
+  <si>
+    <t>servicoController</t>
+  </si>
+  <si>
+    <t>serviceControllerInstance</t>
+  </si>
+  <si>
+    <t>// Instance of  "ServiceTypeController" class</t>
+  </si>
+  <si>
+    <t>getInstanceDeTipoServicoControllerDeveRetornarInstanciaCorrente</t>
+  </si>
+  <si>
+    <t>getInstanceFromServiceTypeController</t>
+  </si>
+  <si>
+    <t>tipoServicoController</t>
+  </si>
+  <si>
+    <t>serviceTypeController</t>
+  </si>
+  <si>
+    <t>// Instances used in the assertion methods</t>
+  </si>
+  <si>
+    <t>inserirDeTipoServicoControllerDeveEnviarUmTipoServico</t>
+  </si>
+  <si>
+    <t>addServiceTypeController</t>
+  </si>
+  <si>
+    <t>excluirDeTipoServicoControllerDeveRemoverUmTipoServico</t>
+  </si>
+  <si>
+    <t>deleteServiceTypeController</t>
+  </si>
+  <si>
+    <t>alterarDeTipoServicoControllerDeveAlterarUmTipoServico</t>
+  </si>
+  <si>
+    <t>editServiceTypeController</t>
+  </si>
+  <si>
+    <t>inserirTipoServicoNaoPodePassarTipoServicoNullo</t>
+  </si>
+  <si>
+    <t>addNotNullServiceType</t>
+  </si>
+  <si>
+    <t>excluirTipoServicoNaoPodePassarTipoServicoNullo</t>
+  </si>
+  <si>
+    <t>deleteNotNullServiceType</t>
+  </si>
+  <si>
+    <t>alterarTipoServicoNaoPodePassarTipoServicoNullo</t>
+  </si>
+  <si>
+    <t>editNotNullServiceType</t>
+  </si>
+  <si>
+    <t>pesquisarPorNomeDeTipoServicoControllerDeveMostrarUmServico</t>
+  </si>
+  <si>
+    <t>searchByServiceTypeNameController</t>
+  </si>
+  <si>
+    <t>Instance used in the assertion method</t>
   </si>
 </sst>
 </file>
@@ -628,7 +1069,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -688,11 +1129,285 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="3" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="3" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3" tint="-0.249977111117893"/>
+      </left>
+      <right style="medium">
+        <color theme="3" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3" tint="-0.249977111117893"/>
+      </left>
+      <right style="medium">
+        <color theme="3" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3" tint="-0.249977111117893"/>
+      </left>
+      <right style="medium">
+        <color theme="3" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3" tint="-0.249977111117893"/>
+      </left>
+      <right style="medium">
+        <color theme="3" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="3" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="3" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -770,6 +1485,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -782,11 +1500,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1133,10 +1926,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="35" t="s">
         <v>88</v>
       </c>
       <c r="C2" s="4"/>
@@ -1152,8 +1945,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="25"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
@@ -1167,12 +1960,12 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34" t="s">
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="35" t="s">
         <v>93</v>
       </c>
       <c r="E4" s="6" t="s">
@@ -1186,10 +1979,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
       <c r="E5" s="6" t="s">
         <v>12</v>
       </c>
@@ -1201,10 +1994,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
       <c r="E6" s="25" t="s">
         <v>97</v>
       </c>
@@ -1216,12 +2009,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34" t="s">
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="35" t="s">
         <v>95</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -1235,10 +2028,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
       <c r="E8" s="25" t="s">
         <v>103</v>
       </c>
@@ -1250,10 +2043,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="32" t="s">
         <v>107</v>
       </c>
       <c r="C9" s="24"/>
@@ -1269,8 +2062,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
       <c r="C10" s="25"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6" t="s">
@@ -1284,8 +2077,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
       <c r="C11" s="25"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
@@ -1299,8 +2092,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="25"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
@@ -1314,12 +2107,12 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="31" t="s">
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="32" t="s">
         <v>95</v>
       </c>
       <c r="E13" s="6" t="s">
@@ -1333,10 +2126,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
       <c r="E14" s="6" t="s">
         <v>12</v>
       </c>
@@ -1348,12 +2141,12 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="31" t="s">
+      <c r="A15" s="33"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="32" t="s">
         <v>95</v>
       </c>
       <c r="E15" s="6" t="s">
@@ -1367,10 +2160,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
       <c r="E16" s="6" t="s">
         <v>112</v>
       </c>
@@ -1382,10 +2175,10 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
       <c r="E17" s="6" t="s">
         <v>115</v>
       </c>
@@ -1397,10 +2190,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
       <c r="E18" s="6" t="s">
         <v>98</v>
       </c>
@@ -1412,10 +2205,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
       <c r="E19" s="6" t="s">
         <v>103</v>
       </c>
@@ -1427,10 +2220,10 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="32" t="s">
         <v>121</v>
       </c>
       <c r="C20" s="26"/>
@@ -1446,8 +2239,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
-      <c r="B21" s="32"/>
+      <c r="A21" s="33"/>
+      <c r="B21" s="33"/>
       <c r="C21" s="26"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
@@ -1461,8 +2254,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
-      <c r="B22" s="32"/>
+      <c r="A22" s="33"/>
+      <c r="B22" s="33"/>
       <c r="C22" s="26"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6" t="s">
@@ -1476,8 +2269,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
-      <c r="B23" s="32"/>
+      <c r="A23" s="33"/>
+      <c r="B23" s="33"/>
       <c r="C23" s="26"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6" t="s">
@@ -1491,8 +2284,8 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
-      <c r="B24" s="32"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
       <c r="C24" s="26"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6" t="s">
@@ -1506,8 +2299,8 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="32"/>
-      <c r="B25" s="32"/>
+      <c r="A25" s="33"/>
+      <c r="B25" s="33"/>
       <c r="C25" s="26"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6" t="s">
@@ -1521,8 +2314,8 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
-      <c r="B26" s="32"/>
+      <c r="A26" s="33"/>
+      <c r="B26" s="33"/>
       <c r="C26" s="26"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6" t="s">
@@ -1536,8 +2329,8 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="32"/>
-      <c r="B27" s="32"/>
+      <c r="A27" s="33"/>
+      <c r="B27" s="33"/>
       <c r="C27" s="26"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6" t="s">
@@ -1551,8 +2344,8 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
-      <c r="B28" s="32"/>
+      <c r="A28" s="33"/>
+      <c r="B28" s="33"/>
       <c r="C28" s="26"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6" t="s">
@@ -1566,12 +2359,12 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="31" t="s">
+      <c r="A29" s="33"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="D29" s="31" t="s">
+      <c r="D29" s="32" t="s">
         <v>121</v>
       </c>
       <c r="E29" s="6" t="s">
@@ -1585,10 +2378,10 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
       <c r="E30" s="6" t="s">
         <v>98</v>
       </c>
@@ -1600,10 +2393,10 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
       <c r="E31" s="6" t="s">
         <v>145</v>
       </c>
@@ -1615,10 +2408,10 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
+      <c r="A32" s="33"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
       <c r="E32" s="6" t="s">
         <v>94</v>
       </c>
@@ -1630,10 +2423,10 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="33"/>
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
+      <c r="A33" s="34"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
       <c r="E33" s="6" t="s">
         <v>147</v>
       </c>
@@ -1838,10 +2631,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B17"/>
+      <selection activeCell="A18" sqref="A18:G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1849,46 +2642,46 @@
     <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="2" width="38.42578125" customWidth="1"/>
     <col min="3" max="3" width="37.7109375" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="4" max="4" width="53.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="42.28515625" customWidth="1"/>
     <col min="6" max="6" width="42.140625" customWidth="1"/>
     <col min="7" max="7" width="98.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="31" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="35" t="s">
         <v>39</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -1902,10 +2695,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
+      <c r="A3" s="35"/>
       <c r="B3" s="36"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
       <c r="E3" s="4" t="s">
         <v>42</v>
       </c>
@@ -1917,10 +2710,10 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="36"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
       <c r="E4" s="4" t="s">
         <v>44</v>
       </c>
@@ -1932,7 +2725,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="36"/>
       <c r="C5" s="30" t="s">
         <v>47</v>
@@ -1951,16 +2744,16 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="35" t="s">
         <v>150</v>
       </c>
       <c r="B6" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="35" t="s">
         <v>152</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -1974,10 +2767,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="36"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
       <c r="E7" s="4" t="s">
         <v>156</v>
       </c>
@@ -1989,10 +2782,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="36"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
       <c r="E8" s="4" t="s">
         <v>159</v>
       </c>
@@ -2004,10 +2797,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="36"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
       <c r="E9" s="28" t="s">
         <v>162</v>
       </c>
@@ -2019,10 +2812,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="36"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
       <c r="E10" s="4" t="s">
         <v>165</v>
       </c>
@@ -2034,10 +2827,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="36"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
       <c r="E11" s="28" t="s">
         <v>168</v>
       </c>
@@ -2049,10 +2842,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="36"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
       <c r="E12" s="28" t="s">
         <v>171</v>
       </c>
@@ -2064,10 +2857,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="36"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
       <c r="E13" s="28" t="s">
         <v>174</v>
       </c>
@@ -2079,10 +2872,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="36"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
       <c r="E14" s="4" t="s">
         <v>176</v>
       </c>
@@ -2094,10 +2887,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
+      <c r="A15" s="35"/>
       <c r="B15" s="36"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
       <c r="E15" s="4" t="s">
         <v>178</v>
       </c>
@@ -2109,10 +2902,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="36"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
       <c r="E16" s="4" t="s">
         <v>145</v>
       </c>
@@ -2124,10 +2917,10 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="36"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
       <c r="E17" s="4" t="s">
         <v>181</v>
       </c>
@@ -2138,8 +2931,1165 @@
         <v>180</v>
       </c>
     </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="B18" s="38" t="s">
+        <v>184</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="D18" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="E18" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="G18" s="40" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="41"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="F19" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="G19" s="40" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="41"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="F20" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="G20" s="40" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="41"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="39" t="s">
+        <v>194</v>
+      </c>
+      <c r="D21" s="39" t="s">
+        <v>195</v>
+      </c>
+      <c r="E21" s="40" t="s">
+        <v>185</v>
+      </c>
+      <c r="F21" s="40" t="s">
+        <v>185</v>
+      </c>
+      <c r="G21" s="40" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="41"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="43" t="s">
+        <v>196</v>
+      </c>
+      <c r="D22" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="E22" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="F22" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="G22" s="40" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="41"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="45" t="s">
+        <v>186</v>
+      </c>
+      <c r="G23" s="45" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="41"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="43" t="s">
+        <v>199</v>
+      </c>
+      <c r="D24" s="43" t="s">
+        <v>200</v>
+      </c>
+      <c r="E24" s="45" t="s">
+        <v>191</v>
+      </c>
+      <c r="F24" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="G24" s="40" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="41"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="G25" s="46" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="41"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="43" t="s">
+        <v>202</v>
+      </c>
+      <c r="D26" s="43" t="s">
+        <v>203</v>
+      </c>
+      <c r="E26" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="F26" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="G26" s="40" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="41"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="G27" s="40" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="41"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="39" t="s">
+        <v>205</v>
+      </c>
+      <c r="D28" s="39" t="s">
+        <v>206</v>
+      </c>
+      <c r="E28" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="F28" s="43" t="s">
+        <v>192</v>
+      </c>
+      <c r="G28" s="40" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="41"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="D29" s="39" t="s">
+        <v>209</v>
+      </c>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="40" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="41"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="43" t="s">
+        <v>211</v>
+      </c>
+      <c r="D30" s="43" t="s">
+        <v>212</v>
+      </c>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="40" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="41"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="G31" s="40" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="41"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="43" t="s">
+        <v>214</v>
+      </c>
+      <c r="D32" s="43" t="s">
+        <v>215</v>
+      </c>
+      <c r="E32" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="F32" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="G32" s="40" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="41"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="G33" s="40" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="41"/>
+      <c r="B34" s="42"/>
+      <c r="C34" s="43" t="s">
+        <v>217</v>
+      </c>
+      <c r="D34" s="43" t="s">
+        <v>218</v>
+      </c>
+      <c r="E34" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="48" t="s">
+        <v>219</v>
+      </c>
+      <c r="G34" s="40" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="41"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="49" t="s">
+        <v>221</v>
+      </c>
+      <c r="G35" s="40" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="41"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="43" t="s">
+        <v>223</v>
+      </c>
+      <c r="D36" s="43" t="s">
+        <v>224</v>
+      </c>
+      <c r="E36" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="40" t="s">
+        <v>219</v>
+      </c>
+      <c r="G36" s="40" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="41"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" s="43" t="s">
+        <v>221</v>
+      </c>
+      <c r="G37" s="40" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="41"/>
+      <c r="B38" s="42"/>
+      <c r="C38" s="43" t="s">
+        <v>226</v>
+      </c>
+      <c r="D38" s="43" t="s">
+        <v>227</v>
+      </c>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="40" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="50"/>
+      <c r="B39" s="51"/>
+      <c r="C39" s="44"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" s="40" t="s">
+        <v>219</v>
+      </c>
+      <c r="G39" s="40" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="B40" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="C40" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="D40" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="E40" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="F40" s="40" t="s">
+        <v>231</v>
+      </c>
+      <c r="G40" s="40" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="41"/>
+      <c r="B41" s="42"/>
+      <c r="C41" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="D41" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="E41" s="44"/>
+      <c r="F41" s="40" t="s">
+        <v>233</v>
+      </c>
+      <c r="G41" s="40" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="41"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="D42" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="E42" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="F42" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="G42" s="40" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="41"/>
+      <c r="B43" s="42"/>
+      <c r="C43" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="D43" s="39" t="s">
+        <v>239</v>
+      </c>
+      <c r="E43" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="F43" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="G43" s="52" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="41"/>
+      <c r="B44" s="42"/>
+      <c r="C44" s="39" t="s">
+        <v>240</v>
+      </c>
+      <c r="D44" s="39" t="s">
+        <v>241</v>
+      </c>
+      <c r="E44" s="47"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="53"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="41"/>
+      <c r="B45" s="42"/>
+      <c r="C45" s="39" t="s">
+        <v>242</v>
+      </c>
+      <c r="D45" s="39" t="s">
+        <v>243</v>
+      </c>
+      <c r="E45" s="44"/>
+      <c r="F45" s="44"/>
+      <c r="G45" s="54"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="41"/>
+      <c r="B46" s="42"/>
+      <c r="C46" s="39" t="s">
+        <v>244</v>
+      </c>
+      <c r="D46" s="39" t="s">
+        <v>245</v>
+      </c>
+      <c r="E46" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="F46" s="40" t="s">
+        <v>246</v>
+      </c>
+      <c r="G46" s="40" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="41"/>
+      <c r="B47" s="42"/>
+      <c r="C47" s="39" t="s">
+        <v>248</v>
+      </c>
+      <c r="D47" s="39" t="s">
+        <v>249</v>
+      </c>
+      <c r="E47" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="F47" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="G47" s="52" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="41"/>
+      <c r="B48" s="42"/>
+      <c r="C48" s="39" t="s">
+        <v>250</v>
+      </c>
+      <c r="D48" s="39" t="s">
+        <v>251</v>
+      </c>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="53"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="41"/>
+      <c r="B49" s="42"/>
+      <c r="C49" s="39" t="s">
+        <v>252</v>
+      </c>
+      <c r="D49" s="39" t="s">
+        <v>253</v>
+      </c>
+      <c r="E49" s="44"/>
+      <c r="F49" s="44"/>
+      <c r="G49" s="54"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="41"/>
+      <c r="B50" s="42"/>
+      <c r="C50" s="39" t="s">
+        <v>254</v>
+      </c>
+      <c r="D50" s="39" t="s">
+        <v>255</v>
+      </c>
+      <c r="E50" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="43" t="s">
+        <v>219</v>
+      </c>
+      <c r="G50" s="52" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="41"/>
+      <c r="B51" s="42"/>
+      <c r="C51" s="39" t="s">
+        <v>256</v>
+      </c>
+      <c r="D51" s="39" t="s">
+        <v>257</v>
+      </c>
+      <c r="E51" s="47"/>
+      <c r="F51" s="47"/>
+      <c r="G51" s="53"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="50"/>
+      <c r="B52" s="51"/>
+      <c r="C52" s="39" t="s">
+        <v>258</v>
+      </c>
+      <c r="D52" s="39" t="s">
+        <v>259</v>
+      </c>
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
+      <c r="G52" s="54"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="55" t="s">
+        <v>260</v>
+      </c>
+      <c r="B53" s="56" t="s">
+        <v>261</v>
+      </c>
+      <c r="C53" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="D53" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="E53" s="43" t="s">
+        <v>262</v>
+      </c>
+      <c r="F53" s="43" t="s">
+        <v>263</v>
+      </c>
+      <c r="G53" s="52" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="58"/>
+      <c r="B54" s="59"/>
+      <c r="C54" s="57" t="s">
+        <v>265</v>
+      </c>
+      <c r="D54" s="39" t="s">
+        <v>266</v>
+      </c>
+      <c r="E54" s="47"/>
+      <c r="F54" s="47"/>
+      <c r="G54" s="53"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="58"/>
+      <c r="B55" s="59"/>
+      <c r="C55" s="57" t="s">
+        <v>267</v>
+      </c>
+      <c r="D55" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="E55" s="47"/>
+      <c r="F55" s="47"/>
+      <c r="G55" s="53"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="58"/>
+      <c r="B56" s="59"/>
+      <c r="C56" s="57" t="s">
+        <v>269</v>
+      </c>
+      <c r="D56" s="39" t="s">
+        <v>270</v>
+      </c>
+      <c r="E56" s="47"/>
+      <c r="F56" s="47"/>
+      <c r="G56" s="53"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="58"/>
+      <c r="B57" s="59"/>
+      <c r="C57" s="57" t="s">
+        <v>271</v>
+      </c>
+      <c r="D57" s="39" t="s">
+        <v>272</v>
+      </c>
+      <c r="E57" s="47"/>
+      <c r="F57" s="47"/>
+      <c r="G57" s="53"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="58"/>
+      <c r="B58" s="59"/>
+      <c r="C58" s="57" t="s">
+        <v>273</v>
+      </c>
+      <c r="D58" s="39" t="s">
+        <v>274</v>
+      </c>
+      <c r="E58" s="47"/>
+      <c r="F58" s="47"/>
+      <c r="G58" s="53"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="58"/>
+      <c r="B59" s="59"/>
+      <c r="C59" s="57" t="s">
+        <v>275</v>
+      </c>
+      <c r="D59" s="39" t="s">
+        <v>276</v>
+      </c>
+      <c r="E59" s="47"/>
+      <c r="F59" s="47"/>
+      <c r="G59" s="53"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="58"/>
+      <c r="B60" s="59"/>
+      <c r="C60" s="57" t="s">
+        <v>277</v>
+      </c>
+      <c r="D60" s="39" t="s">
+        <v>278</v>
+      </c>
+      <c r="E60" s="47"/>
+      <c r="F60" s="47"/>
+      <c r="G60" s="53"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="58"/>
+      <c r="B61" s="59"/>
+      <c r="C61" s="57" t="s">
+        <v>279</v>
+      </c>
+      <c r="D61" s="39" t="s">
+        <v>280</v>
+      </c>
+      <c r="E61" s="44"/>
+      <c r="F61" s="44"/>
+      <c r="G61" s="54"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="58"/>
+      <c r="B62" s="59"/>
+      <c r="C62" s="57" t="s">
+        <v>281</v>
+      </c>
+      <c r="D62" s="39" t="s">
+        <v>282</v>
+      </c>
+      <c r="E62" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="F62" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="G62" s="52" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="58"/>
+      <c r="B63" s="59"/>
+      <c r="C63" s="57" t="s">
+        <v>283</v>
+      </c>
+      <c r="D63" s="39" t="s">
+        <v>284</v>
+      </c>
+      <c r="E63" s="47"/>
+      <c r="F63" s="47"/>
+      <c r="G63" s="53"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="58"/>
+      <c r="B64" s="59"/>
+      <c r="C64" s="57" t="s">
+        <v>285</v>
+      </c>
+      <c r="D64" s="39" t="s">
+        <v>286</v>
+      </c>
+      <c r="E64" s="47"/>
+      <c r="F64" s="47"/>
+      <c r="G64" s="53"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="58"/>
+      <c r="B65" s="59"/>
+      <c r="C65" s="57" t="s">
+        <v>287</v>
+      </c>
+      <c r="D65" s="39" t="s">
+        <v>288</v>
+      </c>
+      <c r="E65" s="44"/>
+      <c r="F65" s="44"/>
+      <c r="G65" s="54"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="58"/>
+      <c r="B66" s="59"/>
+      <c r="C66" s="57" t="s">
+        <v>289</v>
+      </c>
+      <c r="D66" s="39" t="s">
+        <v>290</v>
+      </c>
+      <c r="E66" s="56" t="s">
+        <v>262</v>
+      </c>
+      <c r="F66" s="56" t="s">
+        <v>263</v>
+      </c>
+      <c r="G66" s="56" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="58"/>
+      <c r="B67" s="59"/>
+      <c r="C67" s="57" t="s">
+        <v>292</v>
+      </c>
+      <c r="D67" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="E67" s="59"/>
+      <c r="F67" s="59"/>
+      <c r="G67" s="59"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="58"/>
+      <c r="B68" s="59"/>
+      <c r="C68" s="57" t="s">
+        <v>294</v>
+      </c>
+      <c r="D68" s="39" t="s">
+        <v>295</v>
+      </c>
+      <c r="E68" s="59"/>
+      <c r="F68" s="59"/>
+      <c r="G68" s="59"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="58"/>
+      <c r="B69" s="59"/>
+      <c r="C69" s="57" t="s">
+        <v>296</v>
+      </c>
+      <c r="D69" s="39" t="s">
+        <v>297</v>
+      </c>
+      <c r="E69" s="59"/>
+      <c r="F69" s="59"/>
+      <c r="G69" s="59"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="58"/>
+      <c r="B70" s="59"/>
+      <c r="C70" s="57" t="s">
+        <v>298</v>
+      </c>
+      <c r="D70" s="39" t="s">
+        <v>299</v>
+      </c>
+      <c r="E70" s="59"/>
+      <c r="F70" s="59"/>
+      <c r="G70" s="59"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="58"/>
+      <c r="B71" s="60"/>
+      <c r="C71" s="61" t="s">
+        <v>300</v>
+      </c>
+      <c r="D71" s="61" t="s">
+        <v>301</v>
+      </c>
+      <c r="E71" s="60"/>
+      <c r="F71" s="60"/>
+      <c r="G71" s="60"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="56" t="s">
+        <v>302</v>
+      </c>
+      <c r="B72" s="56" t="s">
+        <v>303</v>
+      </c>
+      <c r="C72" s="56" t="s">
+        <v>185</v>
+      </c>
+      <c r="D72" s="56" t="s">
+        <v>185</v>
+      </c>
+      <c r="E72" s="62" t="s">
+        <v>304</v>
+      </c>
+      <c r="F72" s="62" t="s">
+        <v>305</v>
+      </c>
+      <c r="G72" s="62" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="59"/>
+      <c r="B73" s="59"/>
+      <c r="C73" s="60"/>
+      <c r="D73" s="60"/>
+      <c r="E73" s="62" t="s">
+        <v>307</v>
+      </c>
+      <c r="F73" s="62" t="s">
+        <v>308</v>
+      </c>
+      <c r="G73" s="62" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="59"/>
+      <c r="B74" s="59"/>
+      <c r="C74" s="62" t="s">
+        <v>53</v>
+      </c>
+      <c r="D74" s="62" t="s">
+        <v>185</v>
+      </c>
+      <c r="E74" s="62" t="s">
+        <v>304</v>
+      </c>
+      <c r="F74" s="62" t="s">
+        <v>305</v>
+      </c>
+      <c r="G74" s="62" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="59"/>
+      <c r="B75" s="59"/>
+      <c r="C75" s="56" t="s">
+        <v>310</v>
+      </c>
+      <c r="D75" s="56" t="s">
+        <v>311</v>
+      </c>
+      <c r="E75" s="62" t="s">
+        <v>312</v>
+      </c>
+      <c r="F75" s="62" t="s">
+        <v>313</v>
+      </c>
+      <c r="G75" s="56" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="59"/>
+      <c r="B76" s="59"/>
+      <c r="C76" s="60"/>
+      <c r="D76" s="60"/>
+      <c r="E76" s="56" t="s">
+        <v>307</v>
+      </c>
+      <c r="F76" s="56" t="s">
+        <v>308</v>
+      </c>
+      <c r="G76" s="59"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="59"/>
+      <c r="B77" s="59"/>
+      <c r="C77" s="62" t="s">
+        <v>315</v>
+      </c>
+      <c r="D77" s="62" t="s">
+        <v>316</v>
+      </c>
+      <c r="E77" s="59"/>
+      <c r="F77" s="59"/>
+      <c r="G77" s="59"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="59"/>
+      <c r="B78" s="59"/>
+      <c r="C78" s="62" t="s">
+        <v>317</v>
+      </c>
+      <c r="D78" s="62" t="s">
+        <v>318</v>
+      </c>
+      <c r="E78" s="59"/>
+      <c r="F78" s="59"/>
+      <c r="G78" s="59"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="59"/>
+      <c r="B79" s="59"/>
+      <c r="C79" s="56" t="s">
+        <v>319</v>
+      </c>
+      <c r="D79" s="56" t="s">
+        <v>320</v>
+      </c>
+      <c r="E79" s="60"/>
+      <c r="F79" s="60"/>
+      <c r="G79" s="59"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="59"/>
+      <c r="B80" s="59"/>
+      <c r="C80" s="60"/>
+      <c r="D80" s="60"/>
+      <c r="E80" s="62" t="s">
+        <v>304</v>
+      </c>
+      <c r="F80" s="62" t="s">
+        <v>305</v>
+      </c>
+      <c r="G80" s="59"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="59"/>
+      <c r="B81" s="59"/>
+      <c r="C81" s="62" t="s">
+        <v>321</v>
+      </c>
+      <c r="D81" s="62" t="s">
+        <v>322</v>
+      </c>
+      <c r="E81" s="56" t="s">
+        <v>307</v>
+      </c>
+      <c r="F81" s="56" t="s">
+        <v>308</v>
+      </c>
+      <c r="G81" s="59"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="59"/>
+      <c r="B82" s="59"/>
+      <c r="C82" s="62" t="s">
+        <v>323</v>
+      </c>
+      <c r="D82" s="62" t="s">
+        <v>324</v>
+      </c>
+      <c r="E82" s="59"/>
+      <c r="F82" s="59"/>
+      <c r="G82" s="59"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="59"/>
+      <c r="B83" s="59"/>
+      <c r="C83" s="62" t="s">
+        <v>325</v>
+      </c>
+      <c r="D83" s="62" t="s">
+        <v>326</v>
+      </c>
+      <c r="E83" s="59"/>
+      <c r="F83" s="59"/>
+      <c r="G83" s="59"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="59"/>
+      <c r="B84" s="59"/>
+      <c r="C84" s="56" t="s">
+        <v>256</v>
+      </c>
+      <c r="D84" s="56" t="s">
+        <v>257</v>
+      </c>
+      <c r="E84" s="60"/>
+      <c r="F84" s="60"/>
+      <c r="G84" s="60"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="59"/>
+      <c r="B85" s="59"/>
+      <c r="C85" s="60"/>
+      <c r="D85" s="60"/>
+      <c r="E85" s="56" t="s">
+        <v>12</v>
+      </c>
+      <c r="F85" s="56" t="s">
+        <v>219</v>
+      </c>
+      <c r="G85" s="56" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="59"/>
+      <c r="B86" s="59"/>
+      <c r="C86" s="56" t="s">
+        <v>327</v>
+      </c>
+      <c r="D86" s="56" t="s">
+        <v>328</v>
+      </c>
+      <c r="E86" s="60"/>
+      <c r="F86" s="60"/>
+      <c r="G86" s="60"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="60"/>
+      <c r="B87" s="60"/>
+      <c r="C87" s="60"/>
+      <c r="D87" s="60"/>
+      <c r="E87" s="62" t="s">
+        <v>307</v>
+      </c>
+      <c r="F87" s="62" t="s">
+        <v>308</v>
+      </c>
+      <c r="G87" s="62" t="s">
+        <v>329</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="73">
+    <mergeCell ref="G75:G84"/>
+    <mergeCell ref="E76:E79"/>
+    <mergeCell ref="F76:F79"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="E81:E84"/>
+    <mergeCell ref="F81:F84"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="D84:D85"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="F85:F86"/>
+    <mergeCell ref="G85:G86"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="D86:D87"/>
+    <mergeCell ref="A72:A87"/>
+    <mergeCell ref="B72:B87"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A53:A71"/>
+    <mergeCell ref="B53:B71"/>
+    <mergeCell ref="E53:E61"/>
+    <mergeCell ref="F53:F61"/>
+    <mergeCell ref="G53:G61"/>
+    <mergeCell ref="E62:E65"/>
+    <mergeCell ref="F62:F65"/>
+    <mergeCell ref="G62:G65"/>
+    <mergeCell ref="E66:E71"/>
+    <mergeCell ref="F66:F71"/>
+    <mergeCell ref="G66:G71"/>
+    <mergeCell ref="G43:G45"/>
+    <mergeCell ref="E47:E49"/>
+    <mergeCell ref="F47:F49"/>
+    <mergeCell ref="G47:G49"/>
+    <mergeCell ref="E50:E52"/>
+    <mergeCell ref="F50:F52"/>
+    <mergeCell ref="G50:G52"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="A40:A52"/>
+    <mergeCell ref="B40:B52"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="E43:E45"/>
+    <mergeCell ref="F43:F45"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="F28:F30"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="A18:A39"/>
+    <mergeCell ref="B18:B39"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="C2:C4"/>
@@ -2196,10 +4146,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="32" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="12" t="s">
@@ -2219,8 +4169,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="8" t="s">
         <v>11</v>
       </c>
@@ -2238,8 +4188,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
@@ -2570,16 +4520,16 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="32" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -2593,10 +4543,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
       <c r="E3" s="6" t="s">
         <v>35</v>
       </c>
@@ -2608,8 +4558,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="32"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="18"/>
       <c r="D4" s="19"/>
       <c r="E4" s="7" t="s">
@@ -2623,8 +4573,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="16"/>
       <c r="D5" s="16"/>
     </row>
@@ -2934,16 +4884,16 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="32" t="s">
         <v>48</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -2957,10 +4907,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
       <c r="E3" s="4" t="s">
         <v>57</v>
       </c>
@@ -2972,10 +4922,10 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="6" t="s">
         <v>59</v>
       </c>
@@ -2987,10 +4937,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="6" t="s">
         <v>62</v>
       </c>
@@ -3002,10 +4952,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
       <c r="E6" s="4" t="s">
         <v>64</v>
       </c>
@@ -3017,16 +4967,16 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="32" t="s">
         <v>69</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -3040,10 +4990,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
       <c r="E8" s="6" t="s">
         <v>73</v>
       </c>
@@ -3055,10 +5005,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
       <c r="E9" s="6" t="s">
         <v>76</v>
       </c>
@@ -3070,8 +5020,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
       <c r="C10" s="22" t="s">
         <v>79</v>
       </c>
@@ -3089,16 +5039,16 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="35" t="s">
         <v>86</v>
       </c>
       <c r="E11" s="6" t="s">
@@ -3112,10 +5062,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
       <c r="E12" s="6" t="s">
         <v>59</v>
       </c>

</xml_diff>